<commit_message>
Fix reference file with duplicate styles. Remove Alignment from comparison as it does not exist in cellStyleXfs section.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/CurrentRowColumn.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/CurrentRowColumn.xlsx
@@ -89,13 +89,10 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="9">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -105,20 +102,8 @@
     <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -133,6 +118,10 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -441,8 +430,8 @@
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="14.020625" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="2.900625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <x:col min="2" max="2" width="2.900625" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="9.140625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="15.970625" style="1" customWidth="1"/>
     <x:col min="5" max="5" width="2.900625" style="1" customWidth="1"/>
     <x:col min="6" max="16384" width="9.140625" style="1" customWidth="1"/>
@@ -455,6 +444,7 @@
       <x:c r="B1" s="1" t="n">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="C1" s="1" t="s"/>
       <x:c r="D1" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -469,6 +459,7 @@
       <x:c r="B2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="C2" s="1" t="s"/>
       <x:c r="D2" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -476,28 +467,54 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:5" s="0" customFormat="1">
+      <x:c r="A3" s="1" t="s"/>
+      <x:c r="B3" s="1" t="s"/>
+      <x:c r="C3" s="0" t="s"/>
+      <x:c r="D3" s="1" t="s"/>
+      <x:c r="E3" s="1" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:5" s="0" customFormat="1">
+      <x:c r="A4" s="1" t="s"/>
+      <x:c r="B4" s="1" t="s"/>
+      <x:c r="C4" s="0" t="s"/>
+      <x:c r="D4" s="1" t="s"/>
+      <x:c r="E4" s="1" t="s"/>
+    </x:row>
     <x:row r="5" spans="1:5" s="0" customFormat="1">
-      <x:c r="A5" s="0" t="s"/>
+      <x:c r="A5" s="1" t="s"/>
       <x:c r="B5" s="2" t="s"/>
       <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
+      <x:c r="D5" s="1" t="s"/>
+      <x:c r="E5" s="1" t="s"/>
     </x:row>
     <x:row r="6" spans="1:5" s="0" customFormat="1">
       <x:c r="A6" s="3" t="s"/>
       <x:c r="B6" s="3" t="s"/>
-      <x:c r="C6" s="3" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="B7" s="4" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="B8" s="4" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="B9" s="4" t="s"/>
+      <x:c r="C6" s="4" t="s"/>
+      <x:c r="D6" s="1" t="s"/>
+      <x:c r="E6" s="1" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:5" s="0" customFormat="1">
+      <x:c r="A7" s="0" t="s"/>
+      <x:c r="B7" s="5" t="s"/>
+      <x:c r="C7" s="0" t="s"/>
+      <x:c r="D7" s="0" t="s"/>
+      <x:c r="E7" s="0" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:5" s="0" customFormat="1">
+      <x:c r="A8" s="0" t="s"/>
+      <x:c r="B8" s="5" t="s"/>
+      <x:c r="C8" s="0" t="s"/>
+      <x:c r="D8" s="0" t="s"/>
+      <x:c r="E8" s="0" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:5" s="0" customFormat="1">
+      <x:c r="A9" s="0" t="s"/>
+      <x:c r="B9" s="5" t="s"/>
+      <x:c r="C9" s="0" t="s"/>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Non-initialized cell excluded from children of XLColumn and XLRow. Reference files updated (cells with default styles excluded)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/CurrentRowColumn.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/CurrentRowColumn.xlsx
@@ -441,7 +441,7 @@
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="14.020625" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="2.900625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="2.900625" style="1" customWidth="1"/>
     <x:col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
     <x:col min="4" max="4" width="15.970625" style="1" customWidth="1"/>
     <x:col min="5" max="5" width="2.900625" style="1" customWidth="1"/>
@@ -476,19 +476,13 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:5" s="0" customFormat="1">
-      <x:c r="A5" s="0" t="s"/>
+    <x:row r="5" spans="1:5">
       <x:c r="B5" s="2" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:5" s="0" customFormat="1">
+    </x:row>
+    <x:row r="6" spans="1:5">
       <x:c r="A6" s="3" t="s"/>
       <x:c r="B6" s="3" t="s"/>
       <x:c r="C6" s="3" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="B7" s="4" t="s"/>

</xml_diff>